<commit_message>
fix bug: #117405, #117407
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
@@ -1479,25 +1479,25 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1524,20 +1524,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="60">
@@ -1625,26 +1625,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>365124</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>87313</xdr:rowOff>
+      <xdr:rowOff>103189</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="楕円 1"/>
+        <xdr:cNvPr id="13" name="楕円 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8445500" y="420688"/>
-          <a:ext cx="476250" cy="198437"/>
+          <a:off x="4587874" y="555627"/>
+          <a:ext cx="508001" cy="246062"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -45249,7 +45249,7 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:K6"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12" customHeight="1"/>
@@ -45265,48 +45265,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="28" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="105"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
+      <c r="A1" s="119"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
       <c r="T1" s="29"/>
       <c r="U1" s="110"/>
       <c r="V1" s="110"/>
       <c r="W1" s="110"/>
     </row>
     <row r="2" spans="1:23" s="28" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="106"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
+      <c r="A2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
       <c r="V2" s="111"/>
       <c r="W2" s="111"/>
     </row>
     <row r="3" spans="1:23" s="28" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
+      <c r="A3" s="122"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
     </row>
     <row r="4" spans="1:23" ht="12" customHeight="1">
       <c r="A4" s="24"/>
@@ -45409,8 +45409,8 @@
       <c r="W7" s="69"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="103"/>
-      <c r="B8" s="104"/>
+      <c r="A8" s="118"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="52"/>
       <c r="D8" s="53"/>
       <c r="E8" s="46"/>
@@ -45436,8 +45436,8 @@
     <row r="9" spans="1:23" ht="12" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="122"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="107"/>
       <c r="E9" s="47"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -45486,8 +45486,8 @@
     <row r="11" spans="1:23" ht="12" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="121"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106"/>
       <c r="E11" s="16"/>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
@@ -45586,8 +45586,8 @@
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="104"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
       <c r="E15" s="16"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
@@ -45686,8 +45686,8 @@
     <row r="19" spans="1:23" ht="12" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="109"/>
-      <c r="D19" s="104"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="109"/>
       <c r="E19" s="49"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
@@ -45736,8 +45736,8 @@
     <row r="21" spans="1:23" s="81" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="119"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="104"/>
       <c r="E21" s="90"/>
       <c r="F21" s="87"/>
       <c r="G21" s="19"/>
@@ -45786,8 +45786,8 @@
     <row r="23" spans="1:23" s="81" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="119"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="104"/>
       <c r="E23" s="90"/>
       <c r="F23" s="30"/>
       <c r="G23" s="33"/>
@@ -45860,21 +45860,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'pj/at/dev/team_G/CMF004_release' into pj/at/dev/team_G/teamG_test1"
This reverts commit 8dc360c7475342c5b7c4950f108b8c94e7d70bd3, reversing
changes made to 4502b566921dfbfdd2ffc516dc4e0349db9d3e2d.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\project\KDR001_release\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\KDR001_develop\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -455,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1020,6 +1020,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1145,7 +1156,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1296,6 +1307,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1347,6 +1361,9 @@
     <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1365,6 +1382,9 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1378,6 +1398,9 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1404,41 +1427,26 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -1461,22 +1469,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -45188,81 +45208,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="9" width="5.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="21" width="5.33203125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" style="84" customWidth="1"/>
-    <col min="23" max="23" width="5.33203125" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="3.1640625" style="2"/>
+    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="9" width="5.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="21" width="5.28515625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" style="88" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="3.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="94"/>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
+      <c r="A1" s="105"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
       <c r="T1" s="24"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="98"/>
-      <c r="W1" s="98"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
     </row>
     <row r="2" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="95"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="85"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="89"/>
     </row>
     <row r="3" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="97"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="V3" s="84"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="V3" s="88"/>
     </row>
     <row r="4" spans="1:23" ht="12" customHeight="1">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="102"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="101"/>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -45279,14 +45299,14 @@
     <row r="5" spans="1:23" ht="12" customHeight="1" thickBot="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="55"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -45302,29 +45322,29 @@
       <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" ht="12" customHeight="1" thickBot="1">
-      <c r="A6" s="103"/>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="69"/>
+      <c r="A6" s="102"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
       <c r="A7" s="4"/>
@@ -45336,24 +45356,24 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="85"/>
+      <c r="Q7" s="85"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="85"/>
+      <c r="U7" s="85"/>
+      <c r="V7" s="85"/>
+      <c r="W7" s="85"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="92"/>
-      <c r="B8" s="93"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
       <c r="E8" s="40"/>
@@ -45361,26 +45381,26 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
-      <c r="S8" s="88"/>
-      <c r="T8" s="88"/>
-      <c r="U8" s="88"/>
-      <c r="V8" s="88"/>
-      <c r="W8" s="88"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="110"/>
+      <c r="U8" s="110"/>
+      <c r="V8" s="110"/>
+      <c r="W8" s="110"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="109"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="41"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -45412,130 +45432,130 @@
       <c r="H10" s="19"/>
       <c r="I10" s="34"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="90"/>
-      <c r="P10" s="90"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="90"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="90"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="112"/>
+      <c r="O10" s="112"/>
+      <c r="P10" s="112"/>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="112"/>
+      <c r="S10" s="112"/>
+      <c r="T10" s="112"/>
+      <c r="U10" s="112"/>
+      <c r="V10" s="112"/>
+      <c r="W10" s="112"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="73"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="66"/>
-      <c r="V11" s="66"/>
-      <c r="W11" s="66"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="67"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="67"/>
+      <c r="W11" s="67"/>
     </row>
     <row r="12" spans="1:23" ht="12" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="50"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="13"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="35"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="88"/>
-      <c r="N12" s="88"/>
-      <c r="O12" s="88"/>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="88"/>
-      <c r="R12" s="88"/>
-      <c r="S12" s="88"/>
-      <c r="T12" s="88"/>
-      <c r="U12" s="88"/>
-      <c r="V12" s="88"/>
-      <c r="W12" s="88"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="110"/>
+      <c r="M12" s="110"/>
+      <c r="N12" s="110"/>
+      <c r="O12" s="110"/>
+      <c r="P12" s="110"/>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="110"/>
+      <c r="S12" s="110"/>
+      <c r="T12" s="110"/>
+      <c r="U12" s="110"/>
+      <c r="V12" s="110"/>
+      <c r="W12" s="110"/>
     </row>
     <row r="13" spans="1:23" ht="12" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="51"/>
       <c r="E13" s="13"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="35"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="66"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="66"/>
-      <c r="W13" s="66"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="67"/>
+      <c r="T13" s="67"/>
+      <c r="U13" s="67"/>
+      <c r="V13" s="67"/>
+      <c r="W13" s="67"/>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="42"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="90"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="90"/>
-      <c r="W14" s="90"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="110"/>
+      <c r="N14" s="110"/>
+      <c r="O14" s="110"/>
+      <c r="P14" s="110"/>
+      <c r="Q14" s="110"/>
+      <c r="R14" s="110"/>
+      <c r="S14" s="110"/>
+      <c r="T14" s="110"/>
+      <c r="U14" s="110"/>
+      <c r="V14" s="110"/>
+      <c r="W14" s="110"/>
     </row>
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="43"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="10"/>
       <c r="J15" s="37"/>
       <c r="K15" s="36"/>
       <c r="L15" s="3"/>
@@ -45554,33 +45574,33 @@
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="52"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="9"/>
       <c r="J16" s="38"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
-      <c r="O16" s="90"/>
-      <c r="P16" s="90"/>
-      <c r="Q16" s="90"/>
-      <c r="R16" s="90"/>
-      <c r="S16" s="90"/>
-      <c r="T16" s="90"/>
-      <c r="U16" s="90"/>
-      <c r="V16" s="90"/>
-      <c r="W16" s="90"/>
+      <c r="K16" s="111"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="112"/>
+      <c r="N16" s="112"/>
+      <c r="O16" s="112"/>
+      <c r="P16" s="112"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="112"/>
+      <c r="T16" s="112"/>
+      <c r="U16" s="112"/>
+      <c r="V16" s="112"/>
+      <c r="W16" s="112"/>
     </row>
     <row r="17" spans="1:23" ht="12" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="13"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -45612,82 +45632,82 @@
       <c r="H18" s="19"/>
       <c r="I18" s="11"/>
       <c r="J18" s="38"/>
-      <c r="K18" s="89"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
+      <c r="K18" s="111"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="112"/>
+      <c r="P18" s="112"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="112"/>
+      <c r="S18" s="112"/>
+      <c r="T18" s="112"/>
+      <c r="U18" s="112"/>
+      <c r="V18" s="112"/>
+      <c r="W18" s="112"/>
     </row>
     <row r="19" spans="1:23" ht="12" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="106"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="96"/>
       <c r="E19" s="43"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="66"/>
-      <c r="N19" s="66"/>
-      <c r="O19" s="66"/>
-      <c r="P19" s="66"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="66"/>
-      <c r="S19" s="66"/>
-      <c r="T19" s="66"/>
-      <c r="U19" s="66"/>
-      <c r="V19" s="66"/>
-      <c r="W19" s="66"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="67"/>
+      <c r="T19" s="67"/>
+      <c r="U19" s="67"/>
+      <c r="V19" s="67"/>
+      <c r="W19" s="67"/>
     </row>
     <row r="20" spans="1:23" ht="12" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="89"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="90"/>
-      <c r="O20" s="90"/>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="90"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="90"/>
-      <c r="W20" s="90"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
+      <c r="N20" s="110"/>
+      <c r="O20" s="110"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="110"/>
+      <c r="S20" s="110"/>
+      <c r="T20" s="110"/>
+      <c r="U20" s="110"/>
+      <c r="V20" s="110"/>
+      <c r="W20" s="110"/>
     </row>
-    <row r="21" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+    <row r="21" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="72"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="74"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="74"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="77"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -45701,43 +45721,43 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
-      <c r="A22" s="67"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="91"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="90"/>
-      <c r="N22" s="90"/>
-      <c r="O22" s="90"/>
-      <c r="P22" s="90"/>
-      <c r="Q22" s="90"/>
-      <c r="R22" s="90"/>
-      <c r="S22" s="90"/>
-      <c r="T22" s="90"/>
-      <c r="U22" s="90"/>
-      <c r="V22" s="90"/>
-      <c r="W22" s="90"/>
+    <row r="22" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="113"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="112"/>
+      <c r="P22" s="112"/>
+      <c r="Q22" s="112"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="112"/>
+      <c r="T22" s="112"/>
+      <c r="U22" s="112"/>
+      <c r="V22" s="112"/>
+      <c r="W22" s="112"/>
     </row>
-    <row r="23" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+    <row r="23" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="73"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="76"/>
       <c r="F23" s="25"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="74"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="77"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -45751,72 +45771,72 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+    <row r="24" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="48"/>
       <c r="D24" s="49"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="62"/>
+      <c r="F24" s="63"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="91"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="90"/>
-      <c r="O24" s="90"/>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="90"/>
-      <c r="R24" s="90"/>
-      <c r="S24" s="90"/>
-      <c r="T24" s="90"/>
-      <c r="U24" s="90"/>
-      <c r="V24" s="90"/>
-      <c r="W24" s="90"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="113"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="112"/>
+      <c r="R24" s="112"/>
+      <c r="S24" s="112"/>
+      <c r="T24" s="112"/>
+      <c r="U24" s="112"/>
+      <c r="V24" s="112"/>
+      <c r="W24" s="112"/>
     </row>
     <row r="25" spans="1:23" ht="12" customHeight="1">
-      <c r="A25" s="82"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="83"/>
-      <c r="Q25" s="83"/>
-      <c r="R25" s="83"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="83"/>
-      <c r="U25" s="83"/>
-      <c r="V25" s="83"/>
-      <c r="W25" s="83"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="87"/>
+      <c r="M25" s="87"/>
+      <c r="N25" s="87"/>
+      <c r="O25" s="87"/>
+      <c r="P25" s="87"/>
+      <c r="Q25" s="87"/>
+      <c r="R25" s="87"/>
+      <c r="S25" s="87"/>
+      <c r="T25" s="87"/>
+      <c r="U25" s="87"/>
+      <c r="V25" s="87"/>
+      <c r="W25" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="U1:W1"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'delivery/release_user' into pj/at/dev/team_G/CMF003_release"
This reverts commit 6a7597c4177fbf3fd69f434890051c2b2b8ca922, reversing
changes made to 96ad18e6bda78f24906a86237ce25acba63ed267.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\project\KDR001_release\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\KDR001_develop\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -455,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1020,6 +1020,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1145,7 +1156,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1296,6 +1307,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1347,6 +1361,9 @@
     <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1365,6 +1382,9 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1378,6 +1398,9 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1404,41 +1427,26 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -1461,22 +1469,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -45188,81 +45208,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="9" width="5.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="21" width="5.33203125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" style="84" customWidth="1"/>
-    <col min="23" max="23" width="5.33203125" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="3.1640625" style="2"/>
+    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="9" width="5.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="21" width="5.28515625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" style="88" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="3.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="94"/>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
+      <c r="A1" s="105"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
       <c r="T1" s="24"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="98"/>
-      <c r="W1" s="98"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
     </row>
     <row r="2" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="95"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="85"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="89"/>
     </row>
     <row r="3" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="97"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="V3" s="84"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="V3" s="88"/>
     </row>
     <row r="4" spans="1:23" ht="12" customHeight="1">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="102"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="101"/>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -45279,14 +45299,14 @@
     <row r="5" spans="1:23" ht="12" customHeight="1" thickBot="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="55"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -45302,29 +45322,29 @@
       <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" ht="12" customHeight="1" thickBot="1">
-      <c r="A6" s="103"/>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="69"/>
+      <c r="A6" s="102"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
       <c r="A7" s="4"/>
@@ -45336,24 +45356,24 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="85"/>
+      <c r="Q7" s="85"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="85"/>
+      <c r="U7" s="85"/>
+      <c r="V7" s="85"/>
+      <c r="W7" s="85"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="92"/>
-      <c r="B8" s="93"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
       <c r="E8" s="40"/>
@@ -45361,26 +45381,26 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
-      <c r="S8" s="88"/>
-      <c r="T8" s="88"/>
-      <c r="U8" s="88"/>
-      <c r="V8" s="88"/>
-      <c r="W8" s="88"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="110"/>
+      <c r="U8" s="110"/>
+      <c r="V8" s="110"/>
+      <c r="W8" s="110"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="109"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="41"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -45412,130 +45432,130 @@
       <c r="H10" s="19"/>
       <c r="I10" s="34"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="90"/>
-      <c r="P10" s="90"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="90"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="90"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="112"/>
+      <c r="O10" s="112"/>
+      <c r="P10" s="112"/>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="112"/>
+      <c r="S10" s="112"/>
+      <c r="T10" s="112"/>
+      <c r="U10" s="112"/>
+      <c r="V10" s="112"/>
+      <c r="W10" s="112"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="73"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="66"/>
-      <c r="V11" s="66"/>
-      <c r="W11" s="66"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="67"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="67"/>
+      <c r="W11" s="67"/>
     </row>
     <row r="12" spans="1:23" ht="12" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="50"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="13"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="35"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="88"/>
-      <c r="N12" s="88"/>
-      <c r="O12" s="88"/>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="88"/>
-      <c r="R12" s="88"/>
-      <c r="S12" s="88"/>
-      <c r="T12" s="88"/>
-      <c r="U12" s="88"/>
-      <c r="V12" s="88"/>
-      <c r="W12" s="88"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="110"/>
+      <c r="M12" s="110"/>
+      <c r="N12" s="110"/>
+      <c r="O12" s="110"/>
+      <c r="P12" s="110"/>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="110"/>
+      <c r="S12" s="110"/>
+      <c r="T12" s="110"/>
+      <c r="U12" s="110"/>
+      <c r="V12" s="110"/>
+      <c r="W12" s="110"/>
     </row>
     <row r="13" spans="1:23" ht="12" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="51"/>
       <c r="E13" s="13"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="35"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="66"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="66"/>
-      <c r="W13" s="66"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="67"/>
+      <c r="T13" s="67"/>
+      <c r="U13" s="67"/>
+      <c r="V13" s="67"/>
+      <c r="W13" s="67"/>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="42"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="90"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="90"/>
-      <c r="W14" s="90"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="110"/>
+      <c r="N14" s="110"/>
+      <c r="O14" s="110"/>
+      <c r="P14" s="110"/>
+      <c r="Q14" s="110"/>
+      <c r="R14" s="110"/>
+      <c r="S14" s="110"/>
+      <c r="T14" s="110"/>
+      <c r="U14" s="110"/>
+      <c r="V14" s="110"/>
+      <c r="W14" s="110"/>
     </row>
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="43"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="10"/>
       <c r="J15" s="37"/>
       <c r="K15" s="36"/>
       <c r="L15" s="3"/>
@@ -45554,33 +45574,33 @@
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="52"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="9"/>
       <c r="J16" s="38"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
-      <c r="O16" s="90"/>
-      <c r="P16" s="90"/>
-      <c r="Q16" s="90"/>
-      <c r="R16" s="90"/>
-      <c r="S16" s="90"/>
-      <c r="T16" s="90"/>
-      <c r="U16" s="90"/>
-      <c r="V16" s="90"/>
-      <c r="W16" s="90"/>
+      <c r="K16" s="111"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="112"/>
+      <c r="N16" s="112"/>
+      <c r="O16" s="112"/>
+      <c r="P16" s="112"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="112"/>
+      <c r="T16" s="112"/>
+      <c r="U16" s="112"/>
+      <c r="V16" s="112"/>
+      <c r="W16" s="112"/>
     </row>
     <row r="17" spans="1:23" ht="12" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="13"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -45612,82 +45632,82 @@
       <c r="H18" s="19"/>
       <c r="I18" s="11"/>
       <c r="J18" s="38"/>
-      <c r="K18" s="89"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
+      <c r="K18" s="111"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="112"/>
+      <c r="P18" s="112"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="112"/>
+      <c r="S18" s="112"/>
+      <c r="T18" s="112"/>
+      <c r="U18" s="112"/>
+      <c r="V18" s="112"/>
+      <c r="W18" s="112"/>
     </row>
     <row r="19" spans="1:23" ht="12" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="106"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="96"/>
       <c r="E19" s="43"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="66"/>
-      <c r="N19" s="66"/>
-      <c r="O19" s="66"/>
-      <c r="P19" s="66"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="66"/>
-      <c r="S19" s="66"/>
-      <c r="T19" s="66"/>
-      <c r="U19" s="66"/>
-      <c r="V19" s="66"/>
-      <c r="W19" s="66"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="67"/>
+      <c r="T19" s="67"/>
+      <c r="U19" s="67"/>
+      <c r="V19" s="67"/>
+      <c r="W19" s="67"/>
     </row>
     <row r="20" spans="1:23" ht="12" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="89"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="90"/>
-      <c r="O20" s="90"/>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="90"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="90"/>
-      <c r="W20" s="90"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
+      <c r="N20" s="110"/>
+      <c r="O20" s="110"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="110"/>
+      <c r="S20" s="110"/>
+      <c r="T20" s="110"/>
+      <c r="U20" s="110"/>
+      <c r="V20" s="110"/>
+      <c r="W20" s="110"/>
     </row>
-    <row r="21" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+    <row r="21" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="72"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="74"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="74"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="77"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -45701,43 +45721,43 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
-      <c r="A22" s="67"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="91"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="90"/>
-      <c r="N22" s="90"/>
-      <c r="O22" s="90"/>
-      <c r="P22" s="90"/>
-      <c r="Q22" s="90"/>
-      <c r="R22" s="90"/>
-      <c r="S22" s="90"/>
-      <c r="T22" s="90"/>
-      <c r="U22" s="90"/>
-      <c r="V22" s="90"/>
-      <c r="W22" s="90"/>
+    <row r="22" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="113"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="112"/>
+      <c r="P22" s="112"/>
+      <c r="Q22" s="112"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="112"/>
+      <c r="T22" s="112"/>
+      <c r="U22" s="112"/>
+      <c r="V22" s="112"/>
+      <c r="W22" s="112"/>
     </row>
-    <row r="23" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+    <row r="23" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="73"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="76"/>
       <c r="F23" s="25"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="74"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="77"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -45751,72 +45771,72 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+    <row r="24" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="48"/>
       <c r="D24" s="49"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="62"/>
+      <c r="F24" s="63"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="91"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="90"/>
-      <c r="O24" s="90"/>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="90"/>
-      <c r="R24" s="90"/>
-      <c r="S24" s="90"/>
-      <c r="T24" s="90"/>
-      <c r="U24" s="90"/>
-      <c r="V24" s="90"/>
-      <c r="W24" s="90"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="113"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="112"/>
+      <c r="R24" s="112"/>
+      <c r="S24" s="112"/>
+      <c r="T24" s="112"/>
+      <c r="U24" s="112"/>
+      <c r="V24" s="112"/>
+      <c r="W24" s="112"/>
     </row>
     <row r="25" spans="1:23" ht="12" customHeight="1">
-      <c r="A25" s="82"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="83"/>
-      <c r="Q25" s="83"/>
-      <c r="R25" s="83"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="83"/>
-      <c r="U25" s="83"/>
-      <c r="V25" s="83"/>
-      <c r="W25" s="83"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="87"/>
+      <c r="M25" s="87"/>
+      <c r="N25" s="87"/>
+      <c r="O25" s="87"/>
+      <c r="P25" s="87"/>
+      <c r="Q25" s="87"/>
+      <c r="R25" s="87"/>
+      <c r="S25" s="87"/>
+      <c r="T25" s="87"/>
+      <c r="U25" s="87"/>
+      <c r="V25" s="87"/>
+      <c r="W25" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="U1:W1"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'pj/at/dev/team_G/CMF004_release' into pj/at/dev/team_G/teamG_test1""
This reverts commit 62d8e2e523dfc37a4eaa797946699a01474cab70.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\KDR001_develop\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\project\KDR001_release\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -455,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1020,17 +1020,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1156,7 +1145,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1307,9 +1296,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1361,9 +1347,6 @@
     <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1382,9 +1365,6 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1398,9 +1378,6 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1427,26 +1404,41 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -1469,34 +1461,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -45208,81 +45188,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="9" width="5.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
-    <col min="11" max="21" width="5.28515625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" style="88" customWidth="1"/>
-    <col min="23" max="23" width="5.28515625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="3.140625" style="2"/>
+    <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="9" width="5.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
+    <col min="11" max="21" width="5.33203125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" style="84" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="3.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="105"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
       <c r="T1" s="24"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
     </row>
     <row r="2" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="106"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="89"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="85"/>
     </row>
     <row r="3" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="V3" s="88"/>
+      <c r="A3" s="97"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="V3" s="84"/>
     </row>
     <row r="4" spans="1:23" ht="12" customHeight="1">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="101"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="102"/>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -45299,14 +45279,14 @@
     <row r="5" spans="1:23" ht="12" customHeight="1" thickBot="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="56"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -45322,29 +45302,29 @@
       <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" ht="12" customHeight="1" thickBot="1">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="71"/>
-      <c r="V6" s="71"/>
-      <c r="W6" s="71"/>
+      <c r="A6" s="103"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
       <c r="A7" s="4"/>
@@ -45356,24 +45336,24 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="85"/>
-      <c r="S7" s="85"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="85"/>
-      <c r="V7" s="85"/>
-      <c r="W7" s="85"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
+      <c r="W7" s="81"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="104"/>
-      <c r="B8" s="96"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="93"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
       <c r="E8" s="40"/>
@@ -45381,26 +45361,26 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="110"/>
-      <c r="S8" s="110"/>
-      <c r="T8" s="110"/>
-      <c r="U8" s="110"/>
-      <c r="V8" s="110"/>
-      <c r="W8" s="110"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="88"/>
+      <c r="U8" s="88"/>
+      <c r="V8" s="88"/>
+      <c r="W8" s="88"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="94"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="109"/>
       <c r="E9" s="41"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -45432,130 +45412,130 @@
       <c r="H10" s="19"/>
       <c r="I10" s="34"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="111"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
-      <c r="N10" s="112"/>
-      <c r="O10" s="112"/>
-      <c r="P10" s="112"/>
-      <c r="Q10" s="112"/>
-      <c r="R10" s="112"/>
-      <c r="S10" s="112"/>
-      <c r="T10" s="112"/>
-      <c r="U10" s="112"/>
-      <c r="V10" s="112"/>
-      <c r="W10" s="112"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="90"/>
+      <c r="Q10" s="90"/>
+      <c r="R10" s="90"/>
+      <c r="S10" s="90"/>
+      <c r="T10" s="90"/>
+      <c r="U10" s="90"/>
+      <c r="V10" s="90"/>
+      <c r="W10" s="90"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="67"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="67"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="67"/>
-      <c r="W11" s="67"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
     </row>
     <row r="12" spans="1:23" ht="12" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="13"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="35"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="110"/>
-      <c r="N12" s="110"/>
-      <c r="O12" s="110"/>
-      <c r="P12" s="110"/>
-      <c r="Q12" s="110"/>
-      <c r="R12" s="110"/>
-      <c r="S12" s="110"/>
-      <c r="T12" s="110"/>
-      <c r="U12" s="110"/>
-      <c r="V12" s="110"/>
-      <c r="W12" s="110"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
+      <c r="Q12" s="88"/>
+      <c r="R12" s="88"/>
+      <c r="S12" s="88"/>
+      <c r="T12" s="88"/>
+      <c r="U12" s="88"/>
+      <c r="V12" s="88"/>
+      <c r="W12" s="88"/>
     </row>
     <row r="13" spans="1:23" ht="12" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="13"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="35"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="67"/>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="67"/>
-      <c r="R13" s="67"/>
-      <c r="S13" s="67"/>
-      <c r="T13" s="67"/>
-      <c r="U13" s="67"/>
-      <c r="V13" s="67"/>
-      <c r="W13" s="67"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="66"/>
+      <c r="V13" s="66"/>
+      <c r="W13" s="66"/>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="42"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="110"/>
-      <c r="N14" s="110"/>
-      <c r="O14" s="110"/>
-      <c r="P14" s="110"/>
-      <c r="Q14" s="110"/>
-      <c r="R14" s="110"/>
-      <c r="S14" s="110"/>
-      <c r="T14" s="110"/>
-      <c r="U14" s="110"/>
-      <c r="V14" s="110"/>
-      <c r="W14" s="110"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="90"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="90"/>
+      <c r="W14" s="90"/>
     </row>
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="10"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="37"/>
       <c r="K15" s="36"/>
       <c r="L15" s="3"/>
@@ -45574,33 +45554,33 @@
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="53"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="9"/>
       <c r="J16" s="38"/>
-      <c r="K16" s="111"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
-      <c r="N16" s="112"/>
-      <c r="O16" s="112"/>
-      <c r="P16" s="112"/>
-      <c r="Q16" s="112"/>
-      <c r="R16" s="112"/>
-      <c r="S16" s="112"/>
-      <c r="T16" s="112"/>
-      <c r="U16" s="112"/>
-      <c r="V16" s="112"/>
-      <c r="W16" s="112"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="90"/>
+      <c r="Q16" s="90"/>
+      <c r="R16" s="90"/>
+      <c r="S16" s="90"/>
+      <c r="T16" s="90"/>
+      <c r="U16" s="90"/>
+      <c r="V16" s="90"/>
+      <c r="W16" s="90"/>
     </row>
     <row r="17" spans="1:23" ht="12" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="13"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -45632,82 +45612,82 @@
       <c r="H18" s="19"/>
       <c r="I18" s="11"/>
       <c r="J18" s="38"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
-      <c r="N18" s="112"/>
-      <c r="O18" s="112"/>
-      <c r="P18" s="112"/>
-      <c r="Q18" s="112"/>
-      <c r="R18" s="112"/>
-      <c r="S18" s="112"/>
-      <c r="T18" s="112"/>
-      <c r="U18" s="112"/>
-      <c r="V18" s="112"/>
-      <c r="W18" s="112"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
     </row>
     <row r="19" spans="1:23" ht="12" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="96"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
       <c r="E19" s="43"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67"/>
-      <c r="O19" s="67"/>
-      <c r="P19" s="67"/>
-      <c r="Q19" s="67"/>
-      <c r="R19" s="67"/>
-      <c r="S19" s="67"/>
-      <c r="T19" s="67"/>
-      <c r="U19" s="67"/>
-      <c r="V19" s="67"/>
-      <c r="W19" s="67"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
+      <c r="U19" s="66"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="66"/>
     </row>
     <row r="20" spans="1:23" ht="12" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="110"/>
-      <c r="M20" s="110"/>
-      <c r="N20" s="110"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="110"/>
-      <c r="Q20" s="110"/>
-      <c r="R20" s="110"/>
-      <c r="S20" s="110"/>
-      <c r="T20" s="110"/>
-      <c r="U20" s="110"/>
-      <c r="V20" s="110"/>
-      <c r="W20" s="110"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="90"/>
+      <c r="Q20" s="90"/>
+      <c r="R20" s="90"/>
+      <c r="S20" s="90"/>
+      <c r="T20" s="90"/>
+      <c r="U20" s="90"/>
+      <c r="V20" s="90"/>
+      <c r="W20" s="90"/>
     </row>
-    <row r="21" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+    <row r="21" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="74"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="72"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="74"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -45721,43 +45701,43 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
-      <c r="A22" s="69"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="112"/>
-      <c r="M22" s="112"/>
-      <c r="N22" s="112"/>
-      <c r="O22" s="112"/>
-      <c r="P22" s="112"/>
-      <c r="Q22" s="112"/>
-      <c r="R22" s="112"/>
-      <c r="S22" s="112"/>
-      <c r="T22" s="112"/>
-      <c r="U22" s="112"/>
-      <c r="V22" s="112"/>
-      <c r="W22" s="112"/>
+    <row r="22" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="90"/>
+      <c r="Q22" s="90"/>
+      <c r="R22" s="90"/>
+      <c r="S22" s="90"/>
+      <c r="T22" s="90"/>
+      <c r="U22" s="90"/>
+      <c r="V22" s="90"/>
+      <c r="W22" s="90"/>
     </row>
-    <row r="23" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+    <row r="23" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="76"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="25"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="74"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -45771,72 +45751,72 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+    <row r="24" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="48"/>
       <c r="D24" s="49"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="63"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="113"/>
-      <c r="L24" s="112"/>
-      <c r="M24" s="112"/>
-      <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="112"/>
-      <c r="R24" s="112"/>
-      <c r="S24" s="112"/>
-      <c r="T24" s="112"/>
-      <c r="U24" s="112"/>
-      <c r="V24" s="112"/>
-      <c r="W24" s="112"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="90"/>
+      <c r="O24" s="90"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="90"/>
+      <c r="R24" s="90"/>
+      <c r="S24" s="90"/>
+      <c r="T24" s="90"/>
+      <c r="U24" s="90"/>
+      <c r="V24" s="90"/>
+      <c r="W24" s="90"/>
     </row>
     <row r="25" spans="1:23" ht="12" customHeight="1">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
-      <c r="O25" s="87"/>
-      <c r="P25" s="87"/>
-      <c r="Q25" s="87"/>
-      <c r="R25" s="87"/>
-      <c r="S25" s="87"/>
-      <c r="T25" s="87"/>
-      <c r="U25" s="87"/>
-      <c r="V25" s="87"/>
-      <c r="W25" s="87"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="83"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="83"/>
+      <c r="Q25" s="83"/>
+      <c r="R25" s="83"/>
+      <c r="S25" s="83"/>
+      <c r="T25" s="83"/>
+      <c r="U25" s="83"/>
+      <c r="V25" s="83"/>
+      <c r="W25" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'delivery/release_user' into pj/at/dev/team_G/CMF003_release""
This reverts commit 394bac90d90d72bca19f6a1055f2ff9663a2d474.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/休暇残数管理票_テンプレート.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\KDR001_develop\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\project\KDR001_release\UniversalK\nts.uk\uk.at\at.ctx\function\nts.uk.ctx.at.function.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -455,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1020,17 +1020,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1156,7 +1145,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1307,9 +1296,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1361,9 +1347,6 @@
     <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1382,9 +1365,6 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1398,9 +1378,6 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1427,26 +1404,41 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -1469,34 +1461,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -45208,81 +45188,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="9" width="5.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
-    <col min="11" max="21" width="5.28515625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" style="88" customWidth="1"/>
-    <col min="23" max="23" width="5.28515625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="3.140625" style="2"/>
+    <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="9" width="5.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
+    <col min="11" max="21" width="5.33203125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" style="84" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="3.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="105"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
       <c r="T1" s="24"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
     </row>
     <row r="2" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="106"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="89"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="85"/>
     </row>
     <row r="3" spans="1:23" s="23" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="V3" s="88"/>
+      <c r="A3" s="97"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="V3" s="84"/>
     </row>
     <row r="4" spans="1:23" ht="12" customHeight="1">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="101"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="102"/>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -45299,14 +45279,14 @@
     <row r="5" spans="1:23" ht="12" customHeight="1" thickBot="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="56"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -45322,29 +45302,29 @@
       <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" ht="12" customHeight="1" thickBot="1">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="71"/>
-      <c r="V6" s="71"/>
-      <c r="W6" s="71"/>
+      <c r="A6" s="103"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
       <c r="A7" s="4"/>
@@ -45356,24 +45336,24 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="85"/>
-      <c r="S7" s="85"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="85"/>
-      <c r="V7" s="85"/>
-      <c r="W7" s="85"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
+      <c r="W7" s="81"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="104"/>
-      <c r="B8" s="96"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="93"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
       <c r="E8" s="40"/>
@@ -45381,26 +45361,26 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="110"/>
-      <c r="S8" s="110"/>
-      <c r="T8" s="110"/>
-      <c r="U8" s="110"/>
-      <c r="V8" s="110"/>
-      <c r="W8" s="110"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="88"/>
+      <c r="U8" s="88"/>
+      <c r="V8" s="88"/>
+      <c r="W8" s="88"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="94"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="109"/>
       <c r="E9" s="41"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -45432,130 +45412,130 @@
       <c r="H10" s="19"/>
       <c r="I10" s="34"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="111"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
-      <c r="N10" s="112"/>
-      <c r="O10" s="112"/>
-      <c r="P10" s="112"/>
-      <c r="Q10" s="112"/>
-      <c r="R10" s="112"/>
-      <c r="S10" s="112"/>
-      <c r="T10" s="112"/>
-      <c r="U10" s="112"/>
-      <c r="V10" s="112"/>
-      <c r="W10" s="112"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="90"/>
+      <c r="Q10" s="90"/>
+      <c r="R10" s="90"/>
+      <c r="S10" s="90"/>
+      <c r="T10" s="90"/>
+      <c r="U10" s="90"/>
+      <c r="V10" s="90"/>
+      <c r="W10" s="90"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="67"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="67"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="67"/>
-      <c r="W11" s="67"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
     </row>
     <row r="12" spans="1:23" ht="12" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="13"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="35"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="110"/>
-      <c r="N12" s="110"/>
-      <c r="O12" s="110"/>
-      <c r="P12" s="110"/>
-      <c r="Q12" s="110"/>
-      <c r="R12" s="110"/>
-      <c r="S12" s="110"/>
-      <c r="T12" s="110"/>
-      <c r="U12" s="110"/>
-      <c r="V12" s="110"/>
-      <c r="W12" s="110"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
+      <c r="Q12" s="88"/>
+      <c r="R12" s="88"/>
+      <c r="S12" s="88"/>
+      <c r="T12" s="88"/>
+      <c r="U12" s="88"/>
+      <c r="V12" s="88"/>
+      <c r="W12" s="88"/>
     </row>
     <row r="13" spans="1:23" ht="12" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="13"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="35"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="67"/>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="67"/>
-      <c r="R13" s="67"/>
-      <c r="S13" s="67"/>
-      <c r="T13" s="67"/>
-      <c r="U13" s="67"/>
-      <c r="V13" s="67"/>
-      <c r="W13" s="67"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="66"/>
+      <c r="V13" s="66"/>
+      <c r="W13" s="66"/>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="42"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="110"/>
-      <c r="N14" s="110"/>
-      <c r="O14" s="110"/>
-      <c r="P14" s="110"/>
-      <c r="Q14" s="110"/>
-      <c r="R14" s="110"/>
-      <c r="S14" s="110"/>
-      <c r="T14" s="110"/>
-      <c r="U14" s="110"/>
-      <c r="V14" s="110"/>
-      <c r="W14" s="110"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="90"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="90"/>
+      <c r="W14" s="90"/>
     </row>
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="10"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="37"/>
       <c r="K15" s="36"/>
       <c r="L15" s="3"/>
@@ -45574,33 +45554,33 @@
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="53"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="9"/>
       <c r="J16" s="38"/>
-      <c r="K16" s="111"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
-      <c r="N16" s="112"/>
-      <c r="O16" s="112"/>
-      <c r="P16" s="112"/>
-      <c r="Q16" s="112"/>
-      <c r="R16" s="112"/>
-      <c r="S16" s="112"/>
-      <c r="T16" s="112"/>
-      <c r="U16" s="112"/>
-      <c r="V16" s="112"/>
-      <c r="W16" s="112"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="90"/>
+      <c r="Q16" s="90"/>
+      <c r="R16" s="90"/>
+      <c r="S16" s="90"/>
+      <c r="T16" s="90"/>
+      <c r="U16" s="90"/>
+      <c r="V16" s="90"/>
+      <c r="W16" s="90"/>
     </row>
     <row r="17" spans="1:23" ht="12" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="13"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -45632,82 +45612,82 @@
       <c r="H18" s="19"/>
       <c r="I18" s="11"/>
       <c r="J18" s="38"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
-      <c r="N18" s="112"/>
-      <c r="O18" s="112"/>
-      <c r="P18" s="112"/>
-      <c r="Q18" s="112"/>
-      <c r="R18" s="112"/>
-      <c r="S18" s="112"/>
-      <c r="T18" s="112"/>
-      <c r="U18" s="112"/>
-      <c r="V18" s="112"/>
-      <c r="W18" s="112"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
     </row>
     <row r="19" spans="1:23" ht="12" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="96"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
       <c r="E19" s="43"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67"/>
-      <c r="O19" s="67"/>
-      <c r="P19" s="67"/>
-      <c r="Q19" s="67"/>
-      <c r="R19" s="67"/>
-      <c r="S19" s="67"/>
-      <c r="T19" s="67"/>
-      <c r="U19" s="67"/>
-      <c r="V19" s="67"/>
-      <c r="W19" s="67"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
+      <c r="U19" s="66"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="66"/>
     </row>
     <row r="20" spans="1:23" ht="12" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="110"/>
-      <c r="M20" s="110"/>
-      <c r="N20" s="110"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="110"/>
-      <c r="Q20" s="110"/>
-      <c r="R20" s="110"/>
-      <c r="S20" s="110"/>
-      <c r="T20" s="110"/>
-      <c r="U20" s="110"/>
-      <c r="V20" s="110"/>
-      <c r="W20" s="110"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="90"/>
+      <c r="Q20" s="90"/>
+      <c r="R20" s="90"/>
+      <c r="S20" s="90"/>
+      <c r="T20" s="90"/>
+      <c r="U20" s="90"/>
+      <c r="V20" s="90"/>
+      <c r="W20" s="90"/>
     </row>
-    <row r="21" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+    <row r="21" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="74"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="72"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="74"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -45721,43 +45701,43 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
-      <c r="A22" s="69"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="112"/>
-      <c r="M22" s="112"/>
-      <c r="N22" s="112"/>
-      <c r="O22" s="112"/>
-      <c r="P22" s="112"/>
-      <c r="Q22" s="112"/>
-      <c r="R22" s="112"/>
-      <c r="S22" s="112"/>
-      <c r="T22" s="112"/>
-      <c r="U22" s="112"/>
-      <c r="V22" s="112"/>
-      <c r="W22" s="112"/>
+    <row r="22" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="90"/>
+      <c r="Q22" s="90"/>
+      <c r="R22" s="90"/>
+      <c r="S22" s="90"/>
+      <c r="T22" s="90"/>
+      <c r="U22" s="90"/>
+      <c r="V22" s="90"/>
+      <c r="W22" s="90"/>
     </row>
-    <row r="23" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+    <row r="23" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="76"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="25"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="74"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -45771,72 +45751,72 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" s="70" customFormat="1" ht="12" customHeight="1">
+    <row r="24" spans="1:23" s="68" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="48"/>
       <c r="D24" s="49"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="63"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="113"/>
-      <c r="L24" s="112"/>
-      <c r="M24" s="112"/>
-      <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="112"/>
-      <c r="R24" s="112"/>
-      <c r="S24" s="112"/>
-      <c r="T24" s="112"/>
-      <c r="U24" s="112"/>
-      <c r="V24" s="112"/>
-      <c r="W24" s="112"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="90"/>
+      <c r="O24" s="90"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="90"/>
+      <c r="R24" s="90"/>
+      <c r="S24" s="90"/>
+      <c r="T24" s="90"/>
+      <c r="U24" s="90"/>
+      <c r="V24" s="90"/>
+      <c r="W24" s="90"/>
     </row>
     <row r="25" spans="1:23" ht="12" customHeight="1">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
-      <c r="O25" s="87"/>
-      <c r="P25" s="87"/>
-      <c r="Q25" s="87"/>
-      <c r="R25" s="87"/>
-      <c r="S25" s="87"/>
-      <c r="T25" s="87"/>
-      <c r="U25" s="87"/>
-      <c r="V25" s="87"/>
-      <c r="W25" s="87"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="83"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="83"/>
+      <c r="Q25" s="83"/>
+      <c r="R25" s="83"/>
+      <c r="S25" s="83"/>
+      <c r="T25" s="83"/>
+      <c r="U25" s="83"/>
+      <c r="V25" s="83"/>
+      <c r="W25" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>